<commit_message>
Day 1, designed layout
</commit_message>
<xml_diff>
--- a/bin/nathanDesignDocuments/GANTT Chart TRIVIA GAME (1).xlsx
+++ b/bin/nathanDesignDocuments/GANTT Chart TRIVIA GAME (1).xlsx
@@ -1,12 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B224157C-0AF2-4CC2-A287-9B126DD4D099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="GANTT CHART" sheetId="1" r:id="rId4"/>
+    <sheet name="GANTT CHART" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -52,15 +57,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -71,7 +77,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -93,7 +99,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -107,49 +119,48 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -339,27 +350,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="40.0"/>
-    <col customWidth="1" min="2" max="2" width="8.63"/>
-    <col customWidth="1" min="3" max="5" width="8.5"/>
-    <col customWidth="1" min="6" max="6" width="14.13"/>
-    <col customWidth="1" min="8" max="8" width="15.13"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" customWidth="1"/>
+    <col min="3" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -371,7 +387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -381,8 +397,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="6"/>
@@ -390,15 +406,15 @@
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5"/>
@@ -406,15 +422,15 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="5"/>
@@ -422,15 +438,15 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="6"/>
@@ -438,15 +454,15 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="5"/>
@@ -454,15 +470,15 @@
       <c r="D11" s="6"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="5"/>
@@ -470,27 +486,27 @@
       <c r="D13" s="6"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="5"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>